<commit_message>
fix Shared formulas bug
</commit_message>
<xml_diff>
--- a/src/demo/zxxt_02_excel_xlsx.w3mi.data.xlsx
+++ b/src/demo/zxxt_02_excel_xlsx.w3mi.data.xlsx
@@ -5,36 +5,37 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moldab\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\MoldaB\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8460" tabRatio="703"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="8460" tabRatio="703" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="NoGroup" sheetId="2" r:id="rId1"/>
     <sheet name="ExcelTable" sheetId="4" r:id="rId2"/>
     <sheet name="Pivot based on ExcelTable" sheetId="8" r:id="rId3"/>
-    <sheet name="SimpleTree" sheetId="6" r:id="rId4"/>
-    <sheet name="Tree3" sheetId="7" r:id="rId5"/>
-    <sheet name="PrintArea (8 rows)" sheetId="1" r:id="rId6"/>
+    <sheet name="Formula" sheetId="9" r:id="rId4"/>
+    <sheet name="SimpleTree" sheetId="6" r:id="rId5"/>
+    <sheet name="Tree3" sheetId="7" r:id="rId6"/>
+    <sheet name="PrintArea (8 rows)" sheetId="1" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="E_">Tree3!$E$6</definedName>
     <definedName name="F_">SimpleTree!$F$5</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="5">'PrintArea (8 rows)'!$A$1:$E$8</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">'PrintArea (8 rows)'!$A$1:$E$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">NoGroup!$6:$7</definedName>
     <definedName name="RANGE_SUM1">SimpleTree!$E$5</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="43" r:id="rId7"/>
+    <pivotCache cacheId="4" r:id="rId8"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="36">
   <si>
     <t>Basic table example</t>
   </si>
@@ -138,10 +139,10 @@
     <t>Sum of SUM 2</t>
   </si>
   <si>
-    <t>Months</t>
-  </si>
-  <si>
-    <t>01-Jan</t>
+    <t>Shared formula</t>
+  </si>
+  <si>
+    <t>Specify row number with $ sign</t>
   </si>
 </sst>
 </file>
@@ -517,7 +518,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -699,6 +700,71 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -744,7 +810,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -827,6 +893,37 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -890,7 +987,7 @@
     <dxf>
       <numFmt numFmtId="4" formatCode="#,##0.00"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -899,36 +996,13 @@
         </right>
         <top/>
         <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color auto="1"/>
@@ -957,9 +1031,8 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="4" formatCode="#,##0.00"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color auto="1"/>
         </left>
@@ -968,8 +1041,6 @@
         </right>
         <top/>
         <bottom/>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -990,6 +1061,19 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -1001,6 +1085,19 @@
         <bottom/>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1083,7 +1180,6 @@
   </c:pivotSource>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1304,6 +1400,30 @@
           <c:symbol val="none"/>
         </c:marker>
       </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="13"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="14"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+      </c:pivotFmt>
     </c:pivotFmts>
     <c:plotArea>
       <c:layout/>
@@ -1314,7 +1434,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Pivot based on ExcelTable'!$C$3</c:f>
+              <c:f>'Pivot based on ExcelTable'!$B$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1342,26 +1462,19 @@
             </c:extLst>
           </c:dPt>
           <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>'Pivot based on ExcelTable'!$A$4:$B$5</c:f>
-              <c:multiLvlStrCache>
+            <c:strRef>
+              <c:f>'Pivot based on ExcelTable'!$A$4:$A$5</c:f>
+              <c:strCache>
                 <c:ptCount val="1"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>01-Jan</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Date</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
+                <c:pt idx="0">
+                  <c:v>Date</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pivot based on ExcelTable'!$C$4:$C$5</c:f>
+              <c:f>'Pivot based on ExcelTable'!$B$4:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1382,7 +1495,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Pivot based on ExcelTable'!$D$3</c:f>
+              <c:f>'Pivot based on ExcelTable'!$C$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1410,26 +1523,19 @@
             </c:extLst>
           </c:dPt>
           <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>'Pivot based on ExcelTable'!$A$4:$B$5</c:f>
-              <c:multiLvlStrCache>
+            <c:strRef>
+              <c:f>'Pivot based on ExcelTable'!$A$4:$A$5</c:f>
+              <c:strCache>
                 <c:ptCount val="1"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>01-Jan</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Date</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
+                <c:pt idx="0">
+                  <c:v>Date</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Pivot based on ExcelTable'!$D$4:$D$5</c:f>
+              <c:f>'Pivot based on ExcelTable'!$C$4:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -1466,7 +1572,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2128,11 +2233,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshOnLoad="1" refreshedBy="Moldabayev, Birzhan" refreshedDate="44019.56553738426" missingItemsLimit="0" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshOnLoad="1" refreshedBy="Moldabayev, Birzhan" refreshedDate="44073.360896527774" missingItemsLimit="0" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
-  <cacheFields count="6">
+  <cacheFields count="5">
     <cacheField name="Caption" numFmtId="0">
       <sharedItems count="1">
         <s v="{R-T-CAPTION}"/>
@@ -2142,409 +2247,15 @@
       <sharedItems/>
     </cacheField>
     <cacheField name="Date" numFmtId="14">
-      <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2020-01-01T00:00:00" maxDate="2020-01-02T00:00:00" count="1">
-        <d v="2020-01-01T00:00:00"/>
+      <sharedItems count="1">
+        <s v="{R-T-DATE}"/>
       </sharedItems>
-      <fieldGroup par="5" base="2">
-        <rangePr groupBy="days" startDate="2020-01-01T00:00:00" endDate="2020-01-02T00:00:00"/>
-        <groupItems count="368">
-          <s v="&lt;01/01/2020"/>
-          <s v="01-Jan"/>
-          <s v="02-Jan"/>
-          <s v="03-Jan"/>
-          <s v="04-Jan"/>
-          <s v="05-Jan"/>
-          <s v="06-Jan"/>
-          <s v="07-Jan"/>
-          <s v="08-Jan"/>
-          <s v="09-Jan"/>
-          <s v="10-Jan"/>
-          <s v="11-Jan"/>
-          <s v="12-Jan"/>
-          <s v="13-Jan"/>
-          <s v="14-Jan"/>
-          <s v="15-Jan"/>
-          <s v="16-Jan"/>
-          <s v="17-Jan"/>
-          <s v="18-Jan"/>
-          <s v="19-Jan"/>
-          <s v="20-Jan"/>
-          <s v="21-Jan"/>
-          <s v="22-Jan"/>
-          <s v="23-Jan"/>
-          <s v="24-Jan"/>
-          <s v="25-Jan"/>
-          <s v="26-Jan"/>
-          <s v="27-Jan"/>
-          <s v="28-Jan"/>
-          <s v="29-Jan"/>
-          <s v="30-Jan"/>
-          <s v="31-Jan"/>
-          <s v="01-Feb"/>
-          <s v="02-Feb"/>
-          <s v="03-Feb"/>
-          <s v="04-Feb"/>
-          <s v="05-Feb"/>
-          <s v="06-Feb"/>
-          <s v="07-Feb"/>
-          <s v="08-Feb"/>
-          <s v="09-Feb"/>
-          <s v="10-Feb"/>
-          <s v="11-Feb"/>
-          <s v="12-Feb"/>
-          <s v="13-Feb"/>
-          <s v="14-Feb"/>
-          <s v="15-Feb"/>
-          <s v="16-Feb"/>
-          <s v="17-Feb"/>
-          <s v="18-Feb"/>
-          <s v="19-Feb"/>
-          <s v="20-Feb"/>
-          <s v="21-Feb"/>
-          <s v="22-Feb"/>
-          <s v="23-Feb"/>
-          <s v="24-Feb"/>
-          <s v="25-Feb"/>
-          <s v="26-Feb"/>
-          <s v="27-Feb"/>
-          <s v="28-Feb"/>
-          <s v="29-Feb"/>
-          <s v="01-Mar"/>
-          <s v="02-Mar"/>
-          <s v="03-Mar"/>
-          <s v="04-Mar"/>
-          <s v="05-Mar"/>
-          <s v="06-Mar"/>
-          <s v="07-Mar"/>
-          <s v="08-Mar"/>
-          <s v="09-Mar"/>
-          <s v="10-Mar"/>
-          <s v="11-Mar"/>
-          <s v="12-Mar"/>
-          <s v="13-Mar"/>
-          <s v="14-Mar"/>
-          <s v="15-Mar"/>
-          <s v="16-Mar"/>
-          <s v="17-Mar"/>
-          <s v="18-Mar"/>
-          <s v="19-Mar"/>
-          <s v="20-Mar"/>
-          <s v="21-Mar"/>
-          <s v="22-Mar"/>
-          <s v="23-Mar"/>
-          <s v="24-Mar"/>
-          <s v="25-Mar"/>
-          <s v="26-Mar"/>
-          <s v="27-Mar"/>
-          <s v="28-Mar"/>
-          <s v="29-Mar"/>
-          <s v="30-Mar"/>
-          <s v="31-Mar"/>
-          <s v="01-Apr"/>
-          <s v="02-Apr"/>
-          <s v="03-Apr"/>
-          <s v="04-Apr"/>
-          <s v="05-Apr"/>
-          <s v="06-Apr"/>
-          <s v="07-Apr"/>
-          <s v="08-Apr"/>
-          <s v="09-Apr"/>
-          <s v="10-Apr"/>
-          <s v="11-Apr"/>
-          <s v="12-Apr"/>
-          <s v="13-Apr"/>
-          <s v="14-Apr"/>
-          <s v="15-Apr"/>
-          <s v="16-Apr"/>
-          <s v="17-Apr"/>
-          <s v="18-Apr"/>
-          <s v="19-Apr"/>
-          <s v="20-Apr"/>
-          <s v="21-Apr"/>
-          <s v="22-Apr"/>
-          <s v="23-Apr"/>
-          <s v="24-Apr"/>
-          <s v="25-Apr"/>
-          <s v="26-Apr"/>
-          <s v="27-Apr"/>
-          <s v="28-Apr"/>
-          <s v="29-Apr"/>
-          <s v="30-Apr"/>
-          <s v="01-May"/>
-          <s v="02-May"/>
-          <s v="03-May"/>
-          <s v="04-May"/>
-          <s v="05-May"/>
-          <s v="06-May"/>
-          <s v="07-May"/>
-          <s v="08-May"/>
-          <s v="09-May"/>
-          <s v="10-May"/>
-          <s v="11-May"/>
-          <s v="12-May"/>
-          <s v="13-May"/>
-          <s v="14-May"/>
-          <s v="15-May"/>
-          <s v="16-May"/>
-          <s v="17-May"/>
-          <s v="18-May"/>
-          <s v="19-May"/>
-          <s v="20-May"/>
-          <s v="21-May"/>
-          <s v="22-May"/>
-          <s v="23-May"/>
-          <s v="24-May"/>
-          <s v="25-May"/>
-          <s v="26-May"/>
-          <s v="27-May"/>
-          <s v="28-May"/>
-          <s v="29-May"/>
-          <s v="30-May"/>
-          <s v="31-May"/>
-          <s v="01-Jun"/>
-          <s v="02-Jun"/>
-          <s v="03-Jun"/>
-          <s v="04-Jun"/>
-          <s v="05-Jun"/>
-          <s v="06-Jun"/>
-          <s v="07-Jun"/>
-          <s v="08-Jun"/>
-          <s v="09-Jun"/>
-          <s v="10-Jun"/>
-          <s v="11-Jun"/>
-          <s v="12-Jun"/>
-          <s v="13-Jun"/>
-          <s v="14-Jun"/>
-          <s v="15-Jun"/>
-          <s v="16-Jun"/>
-          <s v="17-Jun"/>
-          <s v="18-Jun"/>
-          <s v="19-Jun"/>
-          <s v="20-Jun"/>
-          <s v="21-Jun"/>
-          <s v="22-Jun"/>
-          <s v="23-Jun"/>
-          <s v="24-Jun"/>
-          <s v="25-Jun"/>
-          <s v="26-Jun"/>
-          <s v="27-Jun"/>
-          <s v="28-Jun"/>
-          <s v="29-Jun"/>
-          <s v="30-Jun"/>
-          <s v="01-Jul"/>
-          <s v="02-Jul"/>
-          <s v="03-Jul"/>
-          <s v="04-Jul"/>
-          <s v="05-Jul"/>
-          <s v="06-Jul"/>
-          <s v="07-Jul"/>
-          <s v="08-Jul"/>
-          <s v="09-Jul"/>
-          <s v="10-Jul"/>
-          <s v="11-Jul"/>
-          <s v="12-Jul"/>
-          <s v="13-Jul"/>
-          <s v="14-Jul"/>
-          <s v="15-Jul"/>
-          <s v="16-Jul"/>
-          <s v="17-Jul"/>
-          <s v="18-Jul"/>
-          <s v="19-Jul"/>
-          <s v="20-Jul"/>
-          <s v="21-Jul"/>
-          <s v="22-Jul"/>
-          <s v="23-Jul"/>
-          <s v="24-Jul"/>
-          <s v="25-Jul"/>
-          <s v="26-Jul"/>
-          <s v="27-Jul"/>
-          <s v="28-Jul"/>
-          <s v="29-Jul"/>
-          <s v="30-Jul"/>
-          <s v="31-Jul"/>
-          <s v="01-Aug"/>
-          <s v="02-Aug"/>
-          <s v="03-Aug"/>
-          <s v="04-Aug"/>
-          <s v="05-Aug"/>
-          <s v="06-Aug"/>
-          <s v="07-Aug"/>
-          <s v="08-Aug"/>
-          <s v="09-Aug"/>
-          <s v="10-Aug"/>
-          <s v="11-Aug"/>
-          <s v="12-Aug"/>
-          <s v="13-Aug"/>
-          <s v="14-Aug"/>
-          <s v="15-Aug"/>
-          <s v="16-Aug"/>
-          <s v="17-Aug"/>
-          <s v="18-Aug"/>
-          <s v="19-Aug"/>
-          <s v="20-Aug"/>
-          <s v="21-Aug"/>
-          <s v="22-Aug"/>
-          <s v="23-Aug"/>
-          <s v="24-Aug"/>
-          <s v="25-Aug"/>
-          <s v="26-Aug"/>
-          <s v="27-Aug"/>
-          <s v="28-Aug"/>
-          <s v="29-Aug"/>
-          <s v="30-Aug"/>
-          <s v="31-Aug"/>
-          <s v="01-Sep"/>
-          <s v="02-Sep"/>
-          <s v="03-Sep"/>
-          <s v="04-Sep"/>
-          <s v="05-Sep"/>
-          <s v="06-Sep"/>
-          <s v="07-Sep"/>
-          <s v="08-Sep"/>
-          <s v="09-Sep"/>
-          <s v="10-Sep"/>
-          <s v="11-Sep"/>
-          <s v="12-Sep"/>
-          <s v="13-Sep"/>
-          <s v="14-Sep"/>
-          <s v="15-Sep"/>
-          <s v="16-Sep"/>
-          <s v="17-Sep"/>
-          <s v="18-Sep"/>
-          <s v="19-Sep"/>
-          <s v="20-Sep"/>
-          <s v="21-Sep"/>
-          <s v="22-Sep"/>
-          <s v="23-Sep"/>
-          <s v="24-Sep"/>
-          <s v="25-Sep"/>
-          <s v="26-Sep"/>
-          <s v="27-Sep"/>
-          <s v="28-Sep"/>
-          <s v="29-Sep"/>
-          <s v="30-Sep"/>
-          <s v="01-Oct"/>
-          <s v="02-Oct"/>
-          <s v="03-Oct"/>
-          <s v="04-Oct"/>
-          <s v="05-Oct"/>
-          <s v="06-Oct"/>
-          <s v="07-Oct"/>
-          <s v="08-Oct"/>
-          <s v="09-Oct"/>
-          <s v="10-Oct"/>
-          <s v="11-Oct"/>
-          <s v="12-Oct"/>
-          <s v="13-Oct"/>
-          <s v="14-Oct"/>
-          <s v="15-Oct"/>
-          <s v="16-Oct"/>
-          <s v="17-Oct"/>
-          <s v="18-Oct"/>
-          <s v="19-Oct"/>
-          <s v="20-Oct"/>
-          <s v="21-Oct"/>
-          <s v="22-Oct"/>
-          <s v="23-Oct"/>
-          <s v="24-Oct"/>
-          <s v="25-Oct"/>
-          <s v="26-Oct"/>
-          <s v="27-Oct"/>
-          <s v="28-Oct"/>
-          <s v="29-Oct"/>
-          <s v="30-Oct"/>
-          <s v="31-Oct"/>
-          <s v="01-Nov"/>
-          <s v="02-Nov"/>
-          <s v="03-Nov"/>
-          <s v="04-Nov"/>
-          <s v="05-Nov"/>
-          <s v="06-Nov"/>
-          <s v="07-Nov"/>
-          <s v="08-Nov"/>
-          <s v="09-Nov"/>
-          <s v="10-Nov"/>
-          <s v="11-Nov"/>
-          <s v="12-Nov"/>
-          <s v="13-Nov"/>
-          <s v="14-Nov"/>
-          <s v="15-Nov"/>
-          <s v="16-Nov"/>
-          <s v="17-Nov"/>
-          <s v="18-Nov"/>
-          <s v="19-Nov"/>
-          <s v="20-Nov"/>
-          <s v="21-Nov"/>
-          <s v="22-Nov"/>
-          <s v="23-Nov"/>
-          <s v="24-Nov"/>
-          <s v="25-Nov"/>
-          <s v="26-Nov"/>
-          <s v="27-Nov"/>
-          <s v="28-Nov"/>
-          <s v="29-Nov"/>
-          <s v="30-Nov"/>
-          <s v="01-Dec"/>
-          <s v="02-Dec"/>
-          <s v="03-Dec"/>
-          <s v="04-Dec"/>
-          <s v="05-Dec"/>
-          <s v="06-Dec"/>
-          <s v="07-Dec"/>
-          <s v="08-Dec"/>
-          <s v="09-Dec"/>
-          <s v="10-Dec"/>
-          <s v="11-Dec"/>
-          <s v="12-Dec"/>
-          <s v="13-Dec"/>
-          <s v="14-Dec"/>
-          <s v="15-Dec"/>
-          <s v="16-Dec"/>
-          <s v="17-Dec"/>
-          <s v="18-Dec"/>
-          <s v="19-Dec"/>
-          <s v="20-Dec"/>
-          <s v="21-Dec"/>
-          <s v="22-Dec"/>
-          <s v="23-Dec"/>
-          <s v="24-Dec"/>
-          <s v="25-Dec"/>
-          <s v="26-Dec"/>
-          <s v="27-Dec"/>
-          <s v="28-Dec"/>
-          <s v="29-Dec"/>
-          <s v="30-Dec"/>
-          <s v="31-Dec"/>
-          <s v="&gt;02/01/2020"/>
-        </groupItems>
-      </fieldGroup>
     </cacheField>
     <cacheField name="SUM 1" numFmtId="4">
       <sharedItems/>
     </cacheField>
     <cacheField name="SUM 2" numFmtId="4">
       <sharedItems/>
-    </cacheField>
-    <cacheField name="Months" numFmtId="0" databaseField="0">
-      <fieldGroup base="2">
-        <rangePr groupBy="months" startDate="2020-01-01T00:00:00" endDate="2020-01-02T00:00:00"/>
-        <groupItems count="14">
-          <s v="&lt;01/01/2020"/>
-          <s v="Jan"/>
-          <s v="Feb"/>
-          <s v="Mar"/>
-          <s v="Apr"/>
-          <s v="May"/>
-          <s v="Jun"/>
-          <s v="Jul"/>
-          <s v="Aug"/>
-          <s v="Sep"/>
-          <s v="Oct"/>
-          <s v="Nov"/>
-          <s v="Dec"/>
-          <s v="&gt;02/01/2020"/>
-        </groupItems>
-      </fieldGroup>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -2556,9 +2267,9 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="43" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1" fieldListSortAscending="1">
-  <location ref="A3:D5" firstHeaderRow="0" firstDataRow="1" firstDataCol="2" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="6">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1" fieldListSortAscending="1">
+  <location ref="A3:C5" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="5">
     <pivotField axis="axisPage" compact="0" outline="0" showAll="0">
       <items count="2">
         <item x="0"/>
@@ -2567,407 +2278,20 @@
     </pivotField>
     <pivotField compact="0" outline="0" showAll="0"/>
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0">
-      <items count="369">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item x="22"/>
-        <item x="23"/>
-        <item x="24"/>
-        <item x="25"/>
-        <item x="26"/>
-        <item x="27"/>
-        <item x="28"/>
-        <item x="29"/>
-        <item x="30"/>
-        <item x="31"/>
-        <item x="32"/>
-        <item x="33"/>
-        <item x="34"/>
-        <item x="35"/>
-        <item x="36"/>
-        <item x="37"/>
-        <item x="38"/>
-        <item x="39"/>
-        <item x="40"/>
-        <item x="41"/>
-        <item x="42"/>
-        <item x="43"/>
-        <item x="44"/>
-        <item x="45"/>
-        <item x="46"/>
-        <item x="47"/>
-        <item x="48"/>
-        <item x="49"/>
-        <item x="50"/>
-        <item x="51"/>
-        <item x="52"/>
-        <item x="53"/>
-        <item x="54"/>
-        <item x="55"/>
-        <item x="56"/>
-        <item x="57"/>
-        <item x="58"/>
-        <item x="59"/>
-        <item x="60"/>
-        <item x="61"/>
-        <item x="62"/>
-        <item x="63"/>
-        <item x="64"/>
-        <item x="65"/>
-        <item x="66"/>
-        <item x="67"/>
-        <item x="68"/>
-        <item x="69"/>
-        <item x="70"/>
-        <item x="71"/>
-        <item x="72"/>
-        <item x="73"/>
-        <item x="74"/>
-        <item x="75"/>
-        <item x="76"/>
-        <item x="77"/>
-        <item x="78"/>
-        <item x="79"/>
-        <item x="80"/>
-        <item x="81"/>
-        <item x="82"/>
-        <item x="83"/>
-        <item x="84"/>
-        <item x="85"/>
-        <item x="86"/>
-        <item x="87"/>
-        <item x="88"/>
-        <item x="89"/>
-        <item x="90"/>
-        <item x="91"/>
-        <item x="92"/>
-        <item x="93"/>
-        <item x="94"/>
-        <item x="95"/>
-        <item x="96"/>
-        <item x="97"/>
-        <item x="98"/>
-        <item x="99"/>
-        <item x="100"/>
-        <item x="101"/>
-        <item x="102"/>
-        <item x="103"/>
-        <item x="104"/>
-        <item x="105"/>
-        <item x="106"/>
-        <item x="107"/>
-        <item x="108"/>
-        <item x="109"/>
-        <item x="110"/>
-        <item x="111"/>
-        <item x="112"/>
-        <item x="113"/>
-        <item x="114"/>
-        <item x="115"/>
-        <item x="116"/>
-        <item x="117"/>
-        <item x="118"/>
-        <item x="119"/>
-        <item x="120"/>
-        <item x="121"/>
-        <item x="122"/>
-        <item x="123"/>
-        <item x="124"/>
-        <item x="125"/>
-        <item x="126"/>
-        <item x="127"/>
-        <item x="128"/>
-        <item x="129"/>
-        <item x="130"/>
-        <item x="131"/>
-        <item x="132"/>
-        <item x="133"/>
-        <item x="134"/>
-        <item x="135"/>
-        <item x="136"/>
-        <item x="137"/>
-        <item x="138"/>
-        <item x="139"/>
-        <item x="140"/>
-        <item x="141"/>
-        <item x="142"/>
-        <item x="143"/>
-        <item x="144"/>
-        <item x="145"/>
-        <item x="146"/>
-        <item x="147"/>
-        <item x="148"/>
-        <item x="149"/>
-        <item x="150"/>
-        <item x="151"/>
-        <item x="152"/>
-        <item x="153"/>
-        <item x="154"/>
-        <item x="155"/>
-        <item x="156"/>
-        <item x="157"/>
-        <item x="158"/>
-        <item x="159"/>
-        <item x="160"/>
-        <item x="161"/>
-        <item x="162"/>
-        <item x="163"/>
-        <item x="164"/>
-        <item x="165"/>
-        <item x="166"/>
-        <item x="167"/>
-        <item x="168"/>
-        <item x="169"/>
-        <item x="170"/>
-        <item x="171"/>
-        <item x="172"/>
-        <item x="173"/>
-        <item x="174"/>
-        <item x="175"/>
-        <item x="176"/>
-        <item x="177"/>
-        <item x="178"/>
-        <item x="179"/>
-        <item x="180"/>
-        <item x="181"/>
-        <item x="182"/>
-        <item x="183"/>
-        <item x="184"/>
-        <item x="185"/>
-        <item x="186"/>
-        <item x="187"/>
-        <item x="188"/>
-        <item x="189"/>
-        <item x="190"/>
-        <item x="191"/>
-        <item x="192"/>
-        <item x="193"/>
-        <item x="194"/>
-        <item x="195"/>
-        <item x="196"/>
-        <item x="197"/>
-        <item x="198"/>
-        <item x="199"/>
-        <item x="200"/>
-        <item x="201"/>
-        <item x="202"/>
-        <item x="203"/>
-        <item x="204"/>
-        <item x="205"/>
-        <item x="206"/>
-        <item x="207"/>
-        <item x="208"/>
-        <item x="209"/>
-        <item x="210"/>
-        <item x="211"/>
-        <item x="212"/>
-        <item x="213"/>
-        <item x="214"/>
-        <item x="215"/>
-        <item x="216"/>
-        <item x="217"/>
-        <item x="218"/>
-        <item x="219"/>
-        <item x="220"/>
-        <item x="221"/>
-        <item x="222"/>
-        <item x="223"/>
-        <item x="224"/>
-        <item x="225"/>
-        <item x="226"/>
-        <item x="227"/>
-        <item x="228"/>
-        <item x="229"/>
-        <item x="230"/>
-        <item x="231"/>
-        <item x="232"/>
-        <item x="233"/>
-        <item x="234"/>
-        <item x="235"/>
-        <item x="236"/>
-        <item x="237"/>
-        <item x="238"/>
-        <item x="239"/>
-        <item x="240"/>
-        <item x="241"/>
-        <item x="242"/>
-        <item x="243"/>
-        <item x="244"/>
-        <item x="245"/>
-        <item x="246"/>
-        <item x="247"/>
-        <item x="248"/>
-        <item x="249"/>
-        <item x="250"/>
-        <item x="251"/>
-        <item x="252"/>
-        <item x="253"/>
-        <item x="254"/>
-        <item x="255"/>
-        <item x="256"/>
-        <item x="257"/>
-        <item x="258"/>
-        <item x="259"/>
-        <item x="260"/>
-        <item x="261"/>
-        <item x="262"/>
-        <item x="263"/>
-        <item x="264"/>
-        <item x="265"/>
-        <item x="266"/>
-        <item x="267"/>
-        <item x="268"/>
-        <item x="269"/>
-        <item x="270"/>
-        <item x="271"/>
-        <item x="272"/>
-        <item x="273"/>
-        <item x="274"/>
-        <item x="275"/>
-        <item x="276"/>
-        <item x="277"/>
-        <item x="278"/>
-        <item x="279"/>
-        <item x="280"/>
-        <item x="281"/>
-        <item x="282"/>
-        <item x="283"/>
-        <item x="284"/>
-        <item x="285"/>
-        <item x="286"/>
-        <item x="287"/>
-        <item x="288"/>
-        <item x="289"/>
-        <item x="290"/>
-        <item x="291"/>
-        <item x="292"/>
-        <item x="293"/>
-        <item x="294"/>
-        <item x="295"/>
-        <item x="296"/>
-        <item x="297"/>
-        <item x="298"/>
-        <item x="299"/>
-        <item x="300"/>
-        <item x="301"/>
-        <item x="302"/>
-        <item x="303"/>
-        <item x="304"/>
-        <item x="305"/>
-        <item x="306"/>
-        <item x="307"/>
-        <item x="308"/>
-        <item x="309"/>
-        <item x="310"/>
-        <item x="311"/>
-        <item x="312"/>
-        <item x="313"/>
-        <item x="314"/>
-        <item x="315"/>
-        <item x="316"/>
-        <item x="317"/>
-        <item x="318"/>
-        <item x="319"/>
-        <item x="320"/>
-        <item x="321"/>
-        <item x="322"/>
-        <item x="323"/>
-        <item x="324"/>
-        <item x="325"/>
-        <item x="326"/>
-        <item x="327"/>
-        <item x="328"/>
-        <item x="329"/>
-        <item x="330"/>
-        <item x="331"/>
-        <item x="332"/>
-        <item x="333"/>
-        <item x="334"/>
-        <item x="335"/>
-        <item x="336"/>
-        <item x="337"/>
-        <item x="338"/>
-        <item x="339"/>
-        <item x="340"/>
-        <item x="341"/>
-        <item x="342"/>
-        <item x="343"/>
-        <item x="344"/>
-        <item x="345"/>
-        <item x="346"/>
-        <item x="347"/>
-        <item x="348"/>
-        <item x="349"/>
-        <item x="350"/>
-        <item x="351"/>
-        <item x="352"/>
-        <item x="353"/>
-        <item x="354"/>
-        <item x="355"/>
-        <item x="356"/>
-        <item x="357"/>
-        <item x="358"/>
-        <item x="359"/>
-        <item x="360"/>
-        <item x="361"/>
-        <item x="362"/>
-        <item x="363"/>
-        <item x="364"/>
-        <item x="365"/>
-        <item x="366"/>
-        <item x="367"/>
+      <items count="2">
+        <item n="Date" x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
     <pivotField dataField="1" compact="0" outline="0" showAll="0"/>
-    <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
-      <items count="14">
-        <item x="0"/>
-        <item n="Date" x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-      </items>
-    </pivotField>
   </pivotFields>
-  <rowFields count="2">
-    <field x="5"/>
+  <rowFields count="1">
     <field x="2"/>
   </rowFields>
   <rowItems count="2">
     <i>
-      <x v="1"/>
-      <x v="1"/>
+      <x/>
     </i>
     <i t="grand">
       <x/>
@@ -2991,7 +2315,7 @@
     <dataField name="Sum of SUM 1" fld="3" baseField="2" baseItem="0"/>
     <dataField name="Sum of SUM 2" fld="4" baseField="2" baseItem="0"/>
   </dataFields>
-  <chartFormats count="2">
+  <chartFormats count="4">
     <chartFormat chart="0" format="11" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
@@ -3010,6 +2334,30 @@
         </references>
       </pivotArea>
     </chartFormat>
+    <chartFormat chart="0" format="13">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="14">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="2" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
   </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -3024,11 +2372,11 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B4:F6" totalsRowCount="1" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10">
   <autoFilter ref="B4:F5"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Caption" totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="4"/>
-    <tableColumn id="2" name="Group" dataDxfId="8" totalsRowDxfId="3"/>
-    <tableColumn id="3" name="Date" dataDxfId="7" totalsRowDxfId="2"/>
-    <tableColumn id="4" name="SUM 1" totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="1"/>
-    <tableColumn id="5" name="SUM 2" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="0"/>
+    <tableColumn id="1" name="Caption" totalsRowLabel="Total" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="2" name="Group" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="3" name="Date" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="4" name="SUM 1" totalsRowFunction="sum" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="5" name="SUM 2" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3333,7 +2681,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+    <sheetView topLeftCell="B5" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
@@ -3426,7 +2774,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3508,7 +2856,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
@@ -3517,12 +2865,12 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="13.42578125" customWidth="1"/>
     <col min="5" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
         <v>1</v>
       </c>
@@ -3530,42 +2878,36 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="32" t="s">
         <v>3</v>
       </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
       <c r="C3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>35</v>
+      <c r="B4" s="33">
+        <v>0</v>
       </c>
       <c r="C4" s="33">
         <v>0</v>
       </c>
-      <c r="D4" s="33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
+      <c r="B5" s="33">
+        <v>0</v>
+      </c>
       <c r="C5" s="33">
-        <v>0</v>
-      </c>
-      <c r="D5" s="33">
         <v>0</v>
       </c>
     </row>
@@ -3577,10 +2919,102 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:I5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40.28515625" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="6" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="40" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="40" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="43"/>
+      <c r="I4" s="44"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="38" t="e">
+        <f>D$5+E$5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G5" s="39">
+        <f>ROW(G$4)</f>
+        <v>4</v>
+      </c>
+      <c r="H5" s="39">
+        <f t="shared" ref="H5:I5" si="0">ROW(H$4)</f>
+        <v>4</v>
+      </c>
+      <c r="I5" s="39">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G4:I4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="F5" evalError="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3680,7 +3114,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -3784,7 +3218,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>

</xml_diff>

<commit_message>
fix bug a template with an image
</commit_message>
<xml_diff>
--- a/src/demo/zxxt_02_excel_xlsx.w3mi.data.xlsx
+++ b/src/demo/zxxt_02_excel_xlsx.w3mi.data.xlsx
@@ -518,7 +518,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -765,6 +765,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -810,7 +821,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -922,6 +933,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2233,7 +2247,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshOnLoad="1" refreshedBy="Moldabayev, Birzhan" refreshedDate="44073.360896527774" missingItemsLimit="0" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshOnLoad="1" refreshedBy="Moldabayev, Birzhan" refreshedDate="44078.483025810187" missingItemsLimit="0" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1">
   <cacheSource type="worksheet">
     <worksheetSource name="Table1"/>
   </cacheSource>
@@ -2919,10 +2933,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I5"/>
+  <dimension ref="A2:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2930,16 +2944,16 @@
     <col min="1" max="1" width="40.28515625" customWidth="1"/>
     <col min="2" max="2" width="35.42578125" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="6" width="12.28515625" customWidth="1"/>
+    <col min="4" max="7" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="40" t="s">
         <v>1</v>
       </c>
@@ -2958,13 +2972,14 @@
       <c r="F4" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="G4" s="42" t="s">
+      <c r="G4" s="45"/>
+      <c r="H4" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="43"/>
-      <c r="I4" s="44"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I4" s="43"/>
+      <c r="J4" s="44"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
         <v>4</v>
       </c>
@@ -2984,22 +2999,26 @@
         <f>D$5+E$5</f>
         <v>#VALUE!</v>
       </c>
-      <c r="G5" s="39">
-        <f>ROW(G$4)</f>
+      <c r="G5" s="38" t="e">
+        <f>D5+E5</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H5" s="39">
+        <f>ROW(H$4)</f>
         <v>4</v>
       </c>
-      <c r="H5" s="39">
-        <f t="shared" ref="H5:I5" si="0">ROW(H$4)</f>
+      <c r="I5" s="39">
+        <f t="shared" ref="I5:J5" si="0">ROW(I$4)</f>
         <v>4</v>
       </c>
-      <c r="I5" s="39">
+      <c r="J5" s="39">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="H4:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>